<commit_message>
Pequenas mudanças no código
</commit_message>
<xml_diff>
--- a/GoogleSheets/bin/Debug/net8.0/TesteParaC#V1.xlsx
+++ b/GoogleSheets/bin/Debug/net8.0/TesteParaC#V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\GoogleSheets\GoogleSheets\bin\Debug\net8.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8D9C7B-46C7-4215-A1CD-A4096AA5ECCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59339A5E-0EBE-426D-85D9-2F62634695EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,34 +36,34 @@
     <t>Idade</t>
   </si>
   <si>
-    <t>Daniel</t>
+    <t>Itqachi</t>
   </si>
   <si>
     <t>Galleazzo</t>
   </si>
   <si>
-    <t>Paulo</t>
-  </si>
-  <si>
-    <t>Júlia</t>
+    <t>sasuke</t>
+  </si>
+  <si>
+    <t>oii</t>
   </si>
   <si>
     <t>Zanon</t>
   </si>
   <si>
-    <t>Sandra</t>
+    <t>Oláaa</t>
   </si>
   <si>
     <t>Antônio</t>
   </si>
   <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Raissa</t>
-  </si>
-  <si>
-    <t>AnticristoSDD</t>
+    <t>Testeee</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Testando</t>
   </si>
 </sst>
 </file>
@@ -429,9 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>